<commit_message>
DOM Change on Prod
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC29_VerifyALL_Links_Myaccount.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC29_VerifyALL_Links_Myaccount.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5242CCCB-9B8E-4A3A-B4CC-8BAD5875CE5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A7B7E9-5470-467D-AA94-6EBE1EC182E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC29_VerifyALL_Links_Myaccount" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="71">
   <si>
     <t>TestCase</t>
   </si>
@@ -234,9 +234,6 @@
   </si>
   <si>
     <t>LoginButton</t>
-  </si>
-  <si>
-    <t>PersonalInfoprofilePageProd</t>
   </si>
 </sst>
 </file>
@@ -666,8 +663,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -879,7 +876,7 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>71</v>
+        <v>44</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>68</v>
@@ -1558,13 +1555,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2116,18 +2113,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2150,18 +2147,18 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>